<commit_message>
Working on board token
</commit_message>
<xml_diff>
--- a/data/MicrotagScan_TokenKey.xlsx
+++ b/data/MicrotagScan_TokenKey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Taylor/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Taylor/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55D19D3-5FCE-5549-ADD2-98BCB04988E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44262B3B-F41D-2A49-9428-67F57109CD36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="2340" windowWidth="27640" windowHeight="16940" xr2:uid="{FB90AAC8-A30D-2940-85FD-3EA0FF56ED81}"/>
+    <workbookView xWindow="19580" yWindow="3520" windowWidth="27640" windowHeight="16940" xr2:uid="{FB90AAC8-A30D-2940-85FD-3EA0FF56ED81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>BNA</t>
+    <t>RPALT</t>
   </si>
   <si>
-    <t>RPA</t>
+    <t>BNAKU</t>
   </si>
 </sst>
 </file>
@@ -393,19 +393,19 @@
   <dimension ref="A2:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="B3:C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1"/>
     </row>

</xml_diff>